<commit_message>
Integração das listas: Artes Visuais, Libras, Intérprete de Libras,Música e Teatro
</commit_message>
<xml_diff>
--- a/teatro_500.xlsx
+++ b/teatro_500.xlsx
@@ -11,175 +11,115 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>DANIELLE PAULA DE JESUS</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>CRISTIANO ANTÔNIO FERNANDES BARBOSA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>MARIA CRISTINA OSCAR BRAGA DE OLIVEIRA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>DENISE MENDES DE GONCALVES</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>GABRIELA MACHADO FERREIRA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>FERNANDA DA SILVEIRA SOUZA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>BIANCA LEITE DE FREITAS</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>MARCOS MONRSI BAVUSO RIBEIRO</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>MARCOS EUDES DA SILVA MOREIRA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>VANDA MARIA FERREIRA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>ALINE HENRIQUES DA SILVA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>DORVINA SANTOS DA CONCEIÇÃO</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>JOYCE NATÁLIA BATISTA LOPES</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>ANA KARLA TZORTZATO ALMEIDA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>EVELINE CINTRA FERRAZ MOREIRA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>MARIANA RAMOS ROSA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>ERIKA ROHLFS PAIVA</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>HERBERT HISCHTER CHAVES DE PAULA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>NAYARA SANTOS FERREIRA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>LICYA DOS SANTOS BENATTI</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>GILBERTO DOS SANTOS ALVES</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>ADSON FRANKLIN DOS SANTOS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>RARUZA KIARA DOS REIS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>ADRIANA CRAVELARI DE MAGALHÃES</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>PAULINE MARA E SILVA DRUMOND</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>LUCYLENA OLIVEIRA QUEIROZ DE PAULA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>SUELY DOS SANTOS CRUZ RODRIGUES</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>MARTHA DO NASCIMENTO LOHSE</t>
     </r>
   </si>
   <si>
@@ -190,7 +130,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="###0;###0"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -206,6 +149,12 @@
       <name val="Times New Roman"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -243,15 +192,15 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -469,12 +418,12 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="30.63"/>
+    <col customWidth="1" min="2" max="2" width="40.13"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1">
-        <v>22.0</v>
+        <v>17.0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -482,7 +431,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <v>1.0</v>
+        <v>18.0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -490,7 +439,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1">
-        <v>2.0</v>
+        <v>19.0</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
@@ -498,7 +447,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1">
-        <v>3.0</v>
+        <v>20.0</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
@@ -506,7 +455,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1">
-        <v>4.0</v>
+        <v>21.0</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
@@ -514,7 +463,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1">
-        <v>5.0</v>
+        <v>22.0</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
@@ -522,7 +471,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1">
-        <v>6.0</v>
+        <v>23.0</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
@@ -530,7 +479,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1">
-        <v>7.0</v>
+        <v>24.0</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>7</v>
@@ -538,7 +487,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1">
-        <v>8.0</v>
+        <v>25.0</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>8</v>
@@ -546,7 +495,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1">
-        <v>9.0</v>
+        <v>26.0</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>9</v>
@@ -554,64 +503,16 @@
     </row>
     <row r="11">
       <c r="A11" s="1">
-        <v>10.0</v>
+        <v>27.0</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1">
-        <v>11.0</v>
-      </c>
-      <c r="B12" s="2" t="s">
+      <c r="A12" s="3"/>
+      <c r="B12" s="4" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1">
-        <v>12.0</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1">
-        <v>13.0</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1">
-        <v>14.0</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1">
-        <v>15.0</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1">
-        <v>16.0</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lista de teatro corrigida
</commit_message>
<xml_diff>
--- a/teatro_500.xlsx
+++ b/teatro_500.xlsx
@@ -11,119 +11,86 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>HERBERT HISCHTER CHAVES DE PAULA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>NAYARA SANTOS FERREIRA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>LICYA DOS SANTOS BENATTI</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>GILBERTO DOS SANTOS ALVES</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>ADSON FRANKLIN DOS SANTOS</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>RARUZA KIARA DOS REIS</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>ADRIANA CRAVELARI DE MAGALHÃES</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>PAULINE MARA E SILVA DRUMOND</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>LUCYLENA OLIVEIRA QUEIROZ DE PAULA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>SUELY DOS SANTOS CRUZ RODRIGUES</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>MARTHA DO NASCIMENTO LOHSE</t>
-    </r>
-  </si>
-  <si>
-    <t>FIM - TEATRO</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>Laura Dominguez Ribeiro</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>Gisela Daher Gerheim</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>Elizabeth Martins De Oliveira</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>Cláudia Daplra Lage</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>Laura Cassiano Silva Mendonça</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>Flávia Da Silva Nascimento</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>Marciley Ribeiro Barbosa</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">FIM - TEATRO </t>
   </si>
 </sst>
 </file>
@@ -133,7 +100,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="###0;###0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -141,20 +108,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <color rgb="FF000009"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
+      <b/>
       <color theme="1"/>
       <name val="Times New Roman"/>
     </font>
     <font>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -188,18 +146,17 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -418,12 +375,12 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="40.13"/>
+    <col customWidth="1" min="2" max="2" width="38.38"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1">
-        <v>17.0</v>
+        <v>28.0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -431,7 +388,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <v>18.0</v>
+        <v>29.0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -439,7 +396,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1">
-        <v>19.0</v>
+        <v>30.0</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
@@ -447,7 +404,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1">
-        <v>20.0</v>
+        <v>31.0</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
@@ -455,7 +412,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1">
-        <v>21.0</v>
+        <v>32.0</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
@@ -463,7 +420,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1">
-        <v>22.0</v>
+        <v>33.0</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
@@ -471,48 +428,15 @@
     </row>
     <row r="7">
       <c r="A7" s="1">
-        <v>23.0</v>
+        <v>34.0</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1">
-        <v>24.0</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1">
-        <v>25.0</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1">
-        <v>26.0</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1">
-        <v>27.0</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>